<commit_message>
This should work, however pptx does not support SVG files. Need PNG (or other file type) examples or to wait for the official ones
</commit_message>
<xml_diff>
--- a/projective_plane.xlsx
+++ b/projective_plane.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -29,6 +29,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -88,8 +89,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -216,31 +221,119 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>0</v>
+      <c r="A1" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
+      <c r="A2" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>